<commit_message>
Revert "Merge branch 'main' into realtime-presence-tracking"
This reverts commit 813f43459ab175d95225611ee91d92e49f017108, reversing
changes made to 1e6738592020c47b7917c686a1a57c32e86f3fa7.
</commit_message>
<xml_diff>
--- a/sprint_planning (version 1).xlsx
+++ b/sprint_planning (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hhhh1\OneDrive\Bureau\SOEN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AEE200-903E-4BD4-BF17-A8E1916CFC42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F87BBC7-15B5-418D-9B5F-66C589496DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="53">
   <si>
     <t>User Story/Task Title</t>
   </si>
@@ -211,36 +211,6 @@
   </si>
   <si>
     <t>ISSUE #</t>
-  </si>
-  <si>
-    <t>US#16 As a user, I want to be able to send and receive direct messages to other users.</t>
-  </si>
-  <si>
-    <t>US#17 As a user, I want to be able to send and receive messages in text channels to communicate with multiple users.</t>
-  </si>
-  <si>
-    <t>US#18 Submit meeting minutes</t>
-  </si>
-  <si>
-    <t>Implement backend messaging logic
-Ensure Encryption and Security
-Implement Real-Time Message Updates
-Implement UI for Selecting a Friend to DM</t>
-  </si>
-  <si>
-    <t>Implement Backend for Sending and Storing Channel Messages
-Implement UI for Sending and Displaying Channel Messages
-Implement Admin Message Moderation (Delete Feature)
-Implement Real-Time Updates for Channel Messages</t>
-  </si>
-  <si>
-    <t>Steven/Mai/Hala</t>
-  </si>
-  <si>
-    <t>Mohamed/Haytham/Shayaan</t>
-  </si>
-  <si>
-    <t>US#19 Project Documentation</t>
   </si>
 </sst>
 </file>
@@ -314,7 +284,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -404,15 +374,6 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -463,7 +424,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,8 +645,8 @@
   </sheetPr>
   <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1045,7 +1006,7 @@
       <c r="F14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="20" t="s">
         <v>16</v>
       </c>
       <c r="H14" s="11" t="s">
@@ -1147,103 +1108,45 @@
       <c r="G18" s="3"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
-        <v>29</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="9">
-        <v>4</v>
-      </c>
-      <c r="D19" s="10">
-        <v>7.3</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="105.6" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
-        <v>33</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="9">
-        <v>6</v>
-      </c>
-      <c r="D20" s="10">
-        <v>7.3</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>59</v>
-      </c>
+    <row r="19" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
-        <v>45</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="9">
-        <v>1</v>
-      </c>
-      <c r="D21" s="10">
-        <v>7.3</v>
-      </c>
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="10"/>
       <c r="E21" s="9"/>
-      <c r="F21" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>50</v>
-      </c>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
-      <c r="B22" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="9">
-        <v>1</v>
-      </c>
-      <c r="D22" s="10">
-        <v>7.3</v>
-      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="10"/>
       <c r="E22" s="9"/>
-      <c r="F22" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22" s="20" t="s">
-        <v>43</v>
-      </c>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
@@ -1650,7 +1553,7 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F48 F31:F46 F3:F17 M15 F19:F29" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F48 F31:F46 F19:F29 F3:F17 M15" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"!,!!,!!!"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G48 G31:G46 G19:G29 N15 F14 G3:G13 G15:G17" xr:uid="{00000000-0002-0000-0000-000001000000}">

</xml_diff>